<commit_message>
Update the app to be more user-friendly.
</commit_message>
<xml_diff>
--- a/data/SampleData_IGGYPOP.xlsx
+++ b/data/SampleData_IGGYPOP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zenanxing/Documents/Exp_Data/TidyBuddy/Tidy-Buddy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1704E1FB-BA64-2448-A96E-1F38EB1EFC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027E87C3-D2A5-0B49-A2AC-4A837AD43956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="760" windowWidth="25820" windowHeight="17880" xr2:uid="{14DBDB46-EC3B-344E-A159-986F3E2C9D53}"/>
+    <workbookView xWindow="-38540" yWindow="780" windowWidth="25820" windowHeight="17880" xr2:uid="{14DBDB46-EC3B-344E-A159-986F3E2C9D53}"/>
   </bookViews>
   <sheets>
     <sheet name="primer_index" sheetId="8" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="122">
   <si>
     <t>A1</t>
   </si>
@@ -359,100 +359,52 @@
     <t>C</t>
   </si>
   <si>
-    <t>5_A01_set323</t>
-  </si>
-  <si>
-    <t>5_A02_set324</t>
-  </si>
-  <si>
-    <t>5_A03_set325</t>
-  </si>
-  <si>
-    <t>5_A04_set326</t>
-  </si>
-  <si>
-    <t>5_A05_set327</t>
-  </si>
-  <si>
-    <t>5_A06_set328</t>
-  </si>
-  <si>
-    <t>5_A07_set329</t>
-  </si>
-  <si>
-    <t>5_A08_set330</t>
-  </si>
-  <si>
-    <t>5_A09_set331</t>
-  </si>
-  <si>
-    <t>5_A10_set332</t>
-  </si>
-  <si>
-    <t>5_A11_set333</t>
-  </si>
-  <si>
-    <t>5_A12_set334</t>
-  </si>
-  <si>
-    <t>5_B01_set335</t>
-  </si>
-  <si>
-    <t>5_B02_set336</t>
-  </si>
-  <si>
-    <t>5_B03_set337</t>
-  </si>
-  <si>
-    <t>5_B04_set338</t>
-  </si>
-  <si>
-    <t>5_B05_set339</t>
-  </si>
-  <si>
-    <t>5_B06_set340</t>
-  </si>
-  <si>
-    <t>5_B07_set341</t>
-  </si>
-  <si>
-    <t>5_B08_set342</t>
-  </si>
-  <si>
-    <t>5_B09_set343</t>
-  </si>
-  <si>
-    <t>5_B10_set344</t>
-  </si>
-  <si>
-    <t>5_B11_set345</t>
-  </si>
-  <si>
-    <t>5_B12_set346</t>
-  </si>
-  <si>
-    <t>5_C01_set347</t>
-  </si>
-  <si>
-    <t>5_C02_set348</t>
-  </si>
-  <si>
-    <t>5_C03_set349</t>
-  </si>
-  <si>
-    <t>5_C04_set350</t>
-  </si>
-  <si>
-    <t>5_C05_set351</t>
-  </si>
-  <si>
-    <t>5_C06_set352</t>
-  </si>
-  <si>
-    <t>5_C07_set353</t>
-  </si>
-  <si>
-    <t>5_C08_set354</t>
+    <t>ind_0001</t>
+  </si>
+  <si>
+    <t>ind_0002</t>
+  </si>
+  <si>
+    <t>ind_0003</t>
+  </si>
+  <si>
+    <t>ind_0004</t>
+  </si>
+  <si>
+    <t>ind_0005</t>
+  </si>
+  <si>
+    <t>ind_0006</t>
+  </si>
+  <si>
+    <t>ind_0007</t>
+  </si>
+  <si>
+    <t>ind_0008</t>
+  </si>
+  <si>
+    <t>ind_0009</t>
+  </si>
+  <si>
+    <t>ind_0010</t>
+  </si>
+  <si>
+    <t>ind_0011</t>
+  </si>
+  <si>
+    <t>ind_0012</t>
+  </si>
+  <si>
+    <t>ind_0013</t>
+  </si>
+  <si>
+    <t>ind_0014</t>
+  </si>
+  <si>
+    <t>ind_0015</t>
+  </si>
+  <si>
+    <t>ind_0016</t>
   </si>
 </sst>
 </file>
@@ -837,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3683CEC9-CC44-CE4A-8743-A9EFA3FC3176}">
-  <dimension ref="A1:CS19"/>
+  <dimension ref="A1:CS21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -894,40 +846,40 @@
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>106</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>106</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
         <v>106</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>107</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" t="s">
         <v>107</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" t="s">
         <v>107</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" t="s">
         <v>107</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" t="s">
         <v>107</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" t="s">
         <v>107</v>
       </c>
       <c r="N2" s="1"/>
@@ -1019,40 +971,40 @@
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>108</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>108</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>108</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" t="s">
         <v>108</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" t="s">
         <v>109</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" t="s">
         <v>109</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" t="s">
         <v>109</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" t="s">
         <v>109</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" t="s">
         <v>109</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1060,40 +1012,40 @@
       <c r="A4" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>110</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" t="s">
         <v>110</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" t="s">
         <v>110</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
         <v>111</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" t="s">
         <v>111</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" t="s">
         <v>111</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" t="s">
         <v>111</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" t="s">
         <v>111</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1101,40 +1053,40 @@
       <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>112</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>112</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" t="s">
         <v>112</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" t="s">
         <v>112</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" t="s">
         <v>113</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" t="s">
         <v>113</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" t="s">
         <v>113</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" t="s">
         <v>113</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" t="s">
         <v>113</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1142,40 +1094,40 @@
       <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>114</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>114</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>114</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>114</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" t="s">
         <v>114</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" t="s">
         <v>114</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" t="s">
         <v>115</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" t="s">
         <v>115</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" t="s">
         <v>115</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" t="s">
         <v>115</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L6" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1183,40 +1135,40 @@
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>116</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>116</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>116</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>116</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" t="s">
         <v>116</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" t="s">
         <v>116</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" t="s">
         <v>117</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" t="s">
         <v>117</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" t="s">
         <v>117</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" t="s">
         <v>117</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" t="s">
         <v>117</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1224,40 +1176,40 @@
       <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>118</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>118</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>118</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>118</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" t="s">
         <v>118</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" t="s">
         <v>118</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" t="s">
         <v>119</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" t="s">
         <v>119</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" t="s">
         <v>119</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" t="s">
         <v>119</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L8" t="s">
         <v>119</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="M8" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1265,40 +1217,40 @@
       <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>120</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>120</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>120</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>120</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" t="s">
         <v>120</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" t="s">
         <v>120</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" t="s">
         <v>121</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" t="s">
         <v>121</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" t="s">
         <v>121</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" t="s">
         <v>121</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L9" t="s">
         <v>121</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="M9" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1347,329 +1299,347 @@
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>123</v>
+      <c r="B12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F12" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I12" t="s">
+        <v>113</v>
+      </c>
+      <c r="J12" t="s">
+        <v>114</v>
+      </c>
+      <c r="K12" t="s">
+        <v>115</v>
+      </c>
+      <c r="L12" t="s">
+        <v>116</v>
+      </c>
+      <c r="M12" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>125</v>
+      <c r="B13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G13" t="s">
+        <v>111</v>
+      </c>
+      <c r="H13" t="s">
+        <v>112</v>
+      </c>
+      <c r="I13" t="s">
+        <v>113</v>
+      </c>
+      <c r="J13" t="s">
+        <v>114</v>
+      </c>
+      <c r="K13" t="s">
+        <v>115</v>
+      </c>
+      <c r="L13" t="s">
+        <v>116</v>
+      </c>
+      <c r="M13" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>105</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>127</v>
+      <c r="B14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F14" t="s">
+        <v>110</v>
+      </c>
+      <c r="G14" t="s">
+        <v>111</v>
+      </c>
+      <c r="H14" t="s">
+        <v>112</v>
+      </c>
+      <c r="I14" t="s">
+        <v>113</v>
+      </c>
+      <c r="J14" t="s">
+        <v>114</v>
+      </c>
+      <c r="K14" t="s">
+        <v>115</v>
+      </c>
+      <c r="L14" t="s">
+        <v>116</v>
+      </c>
+      <c r="M14" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>129</v>
+      <c r="B15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" t="s">
+        <v>107</v>
+      </c>
+      <c r="D15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" t="s">
+        <v>110</v>
+      </c>
+      <c r="G15" t="s">
+        <v>111</v>
+      </c>
+      <c r="H15" t="s">
+        <v>112</v>
+      </c>
+      <c r="I15" t="s">
+        <v>113</v>
+      </c>
+      <c r="J15" t="s">
+        <v>114</v>
+      </c>
+      <c r="K15" t="s">
+        <v>115</v>
+      </c>
+      <c r="L15" t="s">
+        <v>116</v>
+      </c>
+      <c r="M15" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G16" t="s">
+        <v>111</v>
+      </c>
+      <c r="H16" t="s">
+        <v>112</v>
+      </c>
+      <c r="I16" t="s">
+        <v>113</v>
+      </c>
+      <c r="J16" t="s">
+        <v>114</v>
+      </c>
+      <c r="K16" t="s">
+        <v>115</v>
+      </c>
+      <c r="L16" t="s">
+        <v>116</v>
+      </c>
+      <c r="M16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" t="s">
+        <v>110</v>
+      </c>
+      <c r="G17" t="s">
+        <v>111</v>
+      </c>
+      <c r="H17" t="s">
+        <v>112</v>
+      </c>
+      <c r="I17" t="s">
+        <v>113</v>
+      </c>
+      <c r="J17" t="s">
+        <v>114</v>
+      </c>
+      <c r="K17" t="s">
+        <v>115</v>
+      </c>
+      <c r="L17" t="s">
+        <v>116</v>
+      </c>
+      <c r="M17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" t="s">
+        <v>110</v>
+      </c>
+      <c r="G18" t="s">
+        <v>111</v>
+      </c>
+      <c r="H18" t="s">
+        <v>112</v>
+      </c>
+      <c r="I18" t="s">
+        <v>113</v>
+      </c>
+      <c r="J18" t="s">
+        <v>114</v>
+      </c>
+      <c r="K18" t="s">
+        <v>115</v>
+      </c>
+      <c r="L18" t="s">
+        <v>116</v>
+      </c>
+      <c r="M18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>137</v>
-      </c>
+      <c r="B19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G19" t="s">
+        <v>111</v>
+      </c>
+      <c r="H19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I19" t="s">
+        <v>113</v>
+      </c>
+      <c r="J19" t="s">
+        <v>114</v>
+      </c>
+      <c r="K19" t="s">
+        <v>115</v>
+      </c>
+      <c r="L19" t="s">
+        <v>116</v>
+      </c>
+      <c r="M19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1682,7 +1652,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M9"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2105,37 +2075,37 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
       <c r="I12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M12">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -2143,40 +2113,40 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13">
         <v>2</v>
       </c>
       <c r="J13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M13">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -2184,40 +2154,40 @@
         <v>105</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
         <v>3</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G14">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J14">
         <v>3</v>
       </c>
       <c r="K14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M14">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -2225,40 +2195,40 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E15">
         <v>4</v>
       </c>
       <c r="F15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G15">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K15">
         <v>4</v>
       </c>
       <c r="L15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M15">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -2266,40 +2236,40 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F16">
         <v>5</v>
       </c>
       <c r="G16">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L16">
         <v>5</v>
       </c>
       <c r="M16">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -2307,37 +2277,37 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G17">
         <v>6</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I17">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J17">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M17">
         <v>6</v>
@@ -2348,40 +2318,40 @@
         <v>19</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E18">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F18">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G18">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I18">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J18">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K18">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="L18">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M18">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -2389,40 +2359,40 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E19">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F19">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G19">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I19">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J19">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K19">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L19">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M19">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2435,7 +2405,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:M19"/>
+      <selection activeCell="A10" sqref="A10:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3188,7 +3158,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:M19"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>